<commit_message>
Edit to Scripting template
</commit_message>
<xml_diff>
--- a/HTC_Scripting_Template_v4.xlsx
+++ b/HTC_Scripting_Template_v4.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eribertolopez/Documents/GitHub/Aquarium_HTC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E2A099-64C6-D647-B3EC-7EA96785A6C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21D2025-BAC5-DB4D-BAE0-B9E77C5E0378}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1900" windowWidth="38400" windowHeight="21600" xr2:uid="{72935FC3-A054-E347-8166-6079D9172055}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{72935FC3-A054-E347-8166-6079D9172055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Replicates</t>
   </si>
@@ -90,9 +93,6 @@
     <t>Antibiotic_FinalConcentration</t>
   </si>
   <si>
-    <t>Ampicillin Antibiotic</t>
-  </si>
-  <si>
     <t>0.1_ug/mL</t>
   </si>
   <si>
@@ -102,18 +102,6 @@
     <t>{"reagents": {"Ethanol": {"qty": 70, "units": "percent"} }, "temperature": {"qty": 37, "units": "C"}, "duration": {"qty": 15, "units": "minute"}}</t>
   </si>
   <si>
-    <t>0_nM, 50nM, 75_nM</t>
-  </si>
-  <si>
-    <t>0.1009_ug/mL</t>
-  </si>
-  <si>
-    <t>50nM, 75_nM, 100nM</t>
-  </si>
-  <si>
-    <t>{"starting_condition":{"beta-estradiol": {"final_concentration":["200nM"]} } }</t>
-  </si>
-  <si>
     <t>{"flourescence_control": "positive"}</t>
   </si>
   <si>
@@ -123,16 +111,43 @@
     <t>SC</t>
   </si>
   <si>
-    <t>0nM, 1.6nM, 2.5nM, 4nM, 6.3nM, 10nM, 16nM, 25nM, 40nM, 63nM, 100nM, 200nM</t>
-  </si>
-  <si>
-    <t>TEST_STRAIN</t>
-  </si>
-  <si>
-    <t>HTC_Strain_MATa</t>
-  </si>
-  <si>
-    <t>HTC_Strain_MATAlpha</t>
+    <t>{"growth_control": "negative"}</t>
+  </si>
+  <si>
+    <t>1.6nM, 2.5nM, 4nM, 6.3nM, 10nM, 16nM, 25nM, 40nM, 63nM, 100nM, 200nM</t>
+  </si>
+  <si>
+    <t>Hygromycin B Antibiotic</t>
+  </si>
+  <si>
+    <t>Strain A</t>
+  </si>
+  <si>
+    <t>Strain D</t>
+  </si>
+  <si>
+    <t>Strain E</t>
+  </si>
+  <si>
+    <t>Strain B</t>
+  </si>
+  <si>
+    <t>Strain F</t>
+  </si>
+  <si>
+    <t>{"growth_control": "positive"}</t>
+  </si>
+  <si>
+    <t>{"staining_control": "negative"}</t>
+  </si>
+  <si>
+    <t>{"staining_control": "positive"}</t>
+  </si>
+  <si>
+    <t>25nM, 50nM, 75nM</t>
+  </si>
+  <si>
+    <t>Strain C</t>
   </si>
 </sst>
 </file>
@@ -188,6 +203,48 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>8</v>
+          </cell>
+          <cell r="B1">
+            <v>1</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>SC</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>{"flourescence_control": "positive"}</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Strain A</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>Yeast Glycerol Stock</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>9</v>
+          </cell>
+          <cell r="G2" t="str">
+            <v>Yeast Glycerol Stock</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA43CC9C-4A5E-C845-A810-8D25623061CE}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,17 +556,17 @@
     <col min="2" max="2" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.33203125" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="115" bestFit="1" customWidth="1"/>
   </cols>
@@ -575,22 +632,19 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="F2" s="1">
-        <v>6390</v>
+        <v>28349</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -601,172 +655,280 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
+      </c>
+      <c r="H3">
+        <v>384419</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F4" s="1">
+        <v>28350</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
       </c>
       <c r="H5">
-        <v>364268</v>
+        <v>384421</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="F6" s="1">
+        <v>28351</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="H6">
-        <v>364270</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="F7" s="1">
+        <v>28352</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1">
-        <v>6390</v>
+        <v>28353</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1">
+        <v>28355</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1">
-        <v>22544</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>